<commit_message>
US20 Test Case Updated
A more specific version is updated in this file.
</commit_message>
<xml_diff>
--- a/SimpCity US20 Test Case.xlsx
+++ b/SimpCity US20 Test Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sem3.2-DevOps\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718952C5-1370-4210-99F0-AE63B3DE6325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E099D11D-C752-4FDC-9EEA-905CAAE65562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="72">
   <si>
     <t>Test Scenarios for SimpCity</t>
   </si>
@@ -232,13 +232,25 @@
 3. Values from "1" to "5"</t>
   </si>
   <si>
-    <t>3. The system shall process the option value inputted accordingly</t>
-  </si>
-  <si>
     <t>In Progress</t>
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>1. The user enters an any value except "0" to "5".</t>
+  </si>
+  <si>
+    <t>2. The user renters the option value "0" when the "Your Choice?" is prompted.</t>
+  </si>
+  <si>
+    <t>3. The users selects the Start New Game option again</t>
+  </si>
+  <si>
+    <t>4. The users enters the value from that is in the configure menu from either "1" to "5"</t>
+  </si>
+  <si>
+    <t>3. The system shall process the option value inputted accordingly. The user expects to see partial output not returning an output or prompt.</t>
   </si>
 </sst>
 </file>
@@ -329,13 +341,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFD0CECE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD0CECE"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -688,7 +700,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
@@ -940,6 +952,18 @@
       <alignment vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -949,29 +973,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1289,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22602A42-1986-4734-8038-194763616F21}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1309,10 +1324,10 @@
   <sheetData>
     <row r="1" spans="1:11" s="10" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26"/>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="95"/>
+      <c r="C1" s="99"/>
       <c r="D1" s="61"/>
       <c r="E1" s="58"/>
       <c r="F1" s="64"/>
@@ -1324,24 +1339,24 @@
     </row>
     <row r="2" spans="1:11" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="57"/>
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="100"/>
+      <c r="C2" s="93"/>
       <c r="D2" s="20"/>
-      <c r="E2" s="102" t="s">
+      <c r="E2" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="100"/>
+      <c r="F2" s="93"/>
       <c r="G2" s="52"/>
-      <c r="H2" s="100" t="s">
+      <c r="H2" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="100"/>
-      <c r="J2" s="102" t="s">
+      <c r="I2" s="93"/>
+      <c r="J2" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="103"/>
+      <c r="K2" s="96"/>
     </row>
     <row r="3" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
@@ -1403,21 +1418,21 @@
         <v>17</v>
       </c>
       <c r="C5" s="89" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" s="46"/>
       <c r="E5" s="44" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="92" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G5" s="41"/>
       <c r="H5" s="44" t="s">
         <v>17</v>
       </c>
       <c r="I5" s="89" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J5" s="63" t="s">
         <v>21</v>
@@ -1453,20 +1468,20 @@
     </row>
     <row r="7" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26"/>
-      <c r="B7" s="101" t="s">
+      <c r="B7" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="101"/>
+      <c r="C7" s="94"/>
       <c r="D7" s="16"/>
-      <c r="E7" s="101" t="s">
+      <c r="E7" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="101"/>
+      <c r="F7" s="94"/>
       <c r="G7" s="41"/>
-      <c r="H7" s="101" t="s">
+      <c r="H7" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="101"/>
+      <c r="I7" s="94"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="26"/>
@@ -1679,14 +1694,14 @@
       <c r="K16" s="18"/>
     </row>
     <row r="17" spans="1:11" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="93">
+      <c r="A17" s="97">
         <v>4</v>
       </c>
-      <c r="B17" s="93" t="s">
+      <c r="B17" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="96" t="s">
-        <v>53</v>
+      <c r="C17" s="102" t="s">
+        <v>67</v>
       </c>
       <c r="D17" s="22" t="s">
         <v>57</v>
@@ -1695,7 +1710,7 @@
         <v>58</v>
       </c>
       <c r="F17" s="32"/>
-      <c r="G17" s="94" t="s">
+      <c r="G17" s="98" t="s">
         <v>45</v>
       </c>
       <c r="H17" s="29"/>
@@ -1704,19 +1719,21 @@
       <c r="K17" s="18"/>
     </row>
     <row r="18" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="93"/>
-      <c r="B18" s="93"/>
-      <c r="C18" s="97"/>
+      <c r="A18" s="97"/>
+      <c r="B18" s="97"/>
+      <c r="C18" s="103" t="s">
+        <v>68</v>
+      </c>
       <c r="D18" s="25" t="s">
         <v>59</v>
       </c>
       <c r="E18" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="98" t="s">
+      <c r="F18" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="93"/>
+      <c r="G18" s="97"/>
       <c r="H18" s="29" t="s">
         <v>61</v>
       </c>
@@ -1725,17 +1742,19 @@
       <c r="K18" s="18"/>
     </row>
     <row r="19" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="93"/>
-      <c r="B19" s="93"/>
-      <c r="C19" s="97"/>
+      <c r="A19" s="97"/>
+      <c r="B19" s="97"/>
+      <c r="C19" s="103" t="s">
+        <v>69</v>
+      </c>
       <c r="D19" s="24" t="s">
         <v>62</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="99"/>
-      <c r="G19" s="93"/>
+      <c r="F19" s="101"/>
+      <c r="G19" s="97"/>
       <c r="H19" s="29" t="s">
         <v>46</v>
       </c>
@@ -1744,17 +1763,19 @@
       <c r="K19" s="18"/>
     </row>
     <row r="20" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="93"/>
-      <c r="B20" s="93"/>
-      <c r="C20" s="97"/>
+      <c r="A20" s="97"/>
+      <c r="B20" s="97"/>
+      <c r="C20" s="104" t="s">
+        <v>70</v>
+      </c>
       <c r="D20" s="24" t="s">
         <v>64</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" s="99"/>
-      <c r="G20" s="93"/>
+        <v>71</v>
+      </c>
+      <c r="F20" s="101"/>
+      <c r="G20" s="97"/>
       <c r="H20" s="29" t="s">
         <v>46</v>
       </c>
@@ -1802,7 +1823,12 @@
       <c r="K23" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="12">
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="G17:G20"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="F18:F20"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="J2:K2"/>
@@ -1810,12 +1836,6 @@
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="G17:G20"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="F18:F20"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H14:J20" xr:uid="{4128DC36-7888-406E-9331-9EDDE928E7BC}">

</xml_diff>

<commit_message>
US20 Test Scenarios TDA
TDA for US20 has been done, please review
</commit_message>
<xml_diff>
--- a/SimpCity US20 Test Case.xlsx
+++ b/SimpCity US20 Test Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sem3.2-DevOps\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F8AA4D-2D09-473F-A6C4-74A65DB99641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA04C30-378F-4569-9376-B7A7E6B13A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
   <si>
     <t>Test Scenarios for SimpCity</t>
   </si>
@@ -192,22 +192,13 @@
     <t>3. The users selects the Start New Game option again</t>
   </si>
   <si>
-    <t>An error was not displayed, the configure menu is printed again</t>
-  </si>
-  <si>
-    <t>An error occurred in the code</t>
-  </si>
-  <si>
-    <t>The user was no brought back to the main menu</t>
-  </si>
-  <si>
     <t>Done</t>
   </si>
   <si>
+    <t>Claris (Approved in GitHub Pull Request)</t>
+  </si>
+  <si>
     <t>condition to go back to the main menu feature</t>
-  </si>
-  <si>
-    <t>Since, it was metion that the input validation is not done yet, hence this test case passed even it never meet  the expected output</t>
   </si>
   <si>
     <t>The returns back to the main menu after the game ends</t>
@@ -261,6 +252,9 @@
   </si>
   <si>
     <t>3. The system will run into error as input validation is not done</t>
+  </si>
+  <si>
+    <t>Since, it was metion that the input validation is not done yet, hence this test case has passed as there is an error seen where by the configure menu is printed again and the turn number increased/</t>
   </si>
 </sst>
 </file>
@@ -717,7 +711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
@@ -796,9 +790,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -993,6 +984,275 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>904527</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>41909</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5520690</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>5088233</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{131D66B6-2AA8-4EE7-9CA0-6400F26C7A4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18871058" y="3316128"/>
+          <a:ext cx="4616163" cy="5031084"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1706562</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4362829</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>5032534</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B466ADA1-05D5-4855-A5B5-D01F7D37C87D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19665156" y="8597895"/>
+          <a:ext cx="2642932" cy="4927764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1478969</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>185719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4875664</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>5050008</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7756BEAC-90C5-4F23-8DDF-220D30547356}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19459495" y="13905061"/>
+          <a:ext cx="3396695" cy="4856669"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1416584</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>131779</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4817089</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>5013213</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F76CCC1-EDA5-4638-9E69-8585A7152366}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19397110" y="19382305"/>
+          <a:ext cx="3400505" cy="4873814"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>772494</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>64937</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5388657</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>5122691</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D32BBE2-9701-4916-9D23-828881A13C6D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18753020" y="24512437"/>
+          <a:ext cx="4616163" cy="5057754"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>451984</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>659330</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5736316</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>4168541</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7270205-162D-46B9-ADC5-EF8FDF736DBE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18432510" y="30303804"/>
+          <a:ext cx="5288142" cy="3505401"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1294,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22602A42-1986-4734-8038-194763616F21}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1314,249 +1574,253 @@
   <sheetData>
     <row r="1" spans="1:11" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21"/>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="60"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="59"/>
       <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:11" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="87" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="85"/>
+      <c r="C2" s="84"/>
       <c r="D2" s="16"/>
-      <c r="E2" s="87" t="s">
+      <c r="E2" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="85"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="85" t="s">
+      <c r="F2" s="84"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="85"/>
-      <c r="J2" s="87" t="s">
+      <c r="I2" s="84"/>
+      <c r="J2" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="88"/>
+      <c r="K2" s="87"/>
     </row>
     <row r="3" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21"/>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="57" t="s">
+      <c r="D3" s="46"/>
+      <c r="E3" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="57" t="s">
+      <c r="G3" s="31"/>
+      <c r="H3" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="38" t="s">
+      <c r="I3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="40" t="s">
+      <c r="J3" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="45" t="s">
+      <c r="K3" s="44" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="43"/>
-      <c r="B4" s="61" t="s">
+      <c r="A4" s="42"/>
+      <c r="B4" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="50" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="12"/>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="84" t="s">
+      <c r="F4" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="68"/>
-      <c r="H4" s="56" t="s">
+      <c r="G4" s="67"/>
+      <c r="H4" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="58"/>
-      <c r="J4" s="54" t="s">
+      <c r="I4" s="57"/>
+      <c r="J4" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="44" t="s">
+      <c r="K4" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="21"/>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="76" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="35" t="s">
+      <c r="C5" s="75" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="36"/>
+      <c r="E5" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="79" t="s">
+      <c r="F5" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="35" t="s">
+      <c r="G5" s="31"/>
+      <c r="H5" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="76" t="s">
+      <c r="I5" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="J5" s="54" t="s">
+      <c r="J5" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="44" t="s">
+      <c r="K5" s="43" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="21"/>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="70">
+      <c r="C6" s="69">
         <v>44538</v>
       </c>
       <c r="D6" s="12"/>
-      <c r="E6" s="71" t="s">
+      <c r="E6" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="70"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="71" t="s">
+      <c r="F6" s="69">
+        <v>44541</v>
+      </c>
+      <c r="G6" s="31"/>
+      <c r="H6" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="68"/>
-      <c r="J6" s="40" t="s">
+      <c r="I6" s="67"/>
+      <c r="J6" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="41" t="s">
+      <c r="K6" s="40" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21"/>
-      <c r="B7" s="86" t="s">
+      <c r="B7" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="86"/>
+      <c r="C7" s="85"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="86" t="s">
+      <c r="E7" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="86"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="86" t="s">
+      <c r="F7" s="85"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="86"/>
+      <c r="I7" s="85"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="21"/>
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="94"/>
+      <c r="C8" s="93" t="s">
+        <v>54</v>
+      </c>
       <c r="D8" s="14"/>
-      <c r="E8" s="74" t="s">
+      <c r="E8" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="73" t="s">
+      <c r="F8" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="38"/>
-      <c r="H8" s="74" t="s">
+      <c r="G8" s="37"/>
+      <c r="H8" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="75" t="s">
+      <c r="I8" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="46"/>
-      <c r="K8" s="47"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="46"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21"/>
-      <c r="B9" s="62"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="72" t="s">
+      <c r="B9" s="61"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="77" t="s">
+      <c r="F9" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="32"/>
-      <c r="H9" s="64" t="s">
+      <c r="G9" s="31"/>
+      <c r="H9" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="36" t="s">
+      <c r="I9" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="32"/>
+      <c r="J9" s="31"/>
       <c r="K9" s="12"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="65"/>
+      <c r="A10" s="64"/>
       <c r="D10" s="3"/>
       <c r="E10" s="1"/>
       <c r="F10" s="25"/>
-      <c r="G10" s="65"/>
-      <c r="H10" s="66" t="s">
+      <c r="G10" s="64"/>
+      <c r="H10" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="36" t="s">
+      <c r="I10" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="32"/>
+      <c r="J10" s="31"/>
       <c r="K10" s="12"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="21"/>
-      <c r="B11" s="63"/>
+      <c r="B11" s="62"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="25"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
       <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="21"/>
       <c r="B12" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="39"/>
+      <c r="G12" s="38"/>
       <c r="H12" s="22"/>
       <c r="I12" s="25"/>
       <c r="J12" s="25"/>
@@ -1592,66 +1856,64 @@
       <c r="H14" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="31" t="s">
+      <c r="I14" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="J14" s="31" t="s">
+      <c r="J14" s="30" t="s">
         <v>37</v>
       </c>
       <c r="K14" s="23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="83">
+    <row r="15" spans="1:11" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="82">
         <v>1</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>62</v>
-      </c>
       <c r="D15" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="83" t="s">
+      <c r="F15" s="82" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="83" t="s">
+      <c r="G15" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="83" t="s">
+      <c r="H15" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="I15" s="83"/>
-      <c r="J15" s="83" t="s">
-        <v>50</v>
-      </c>
-      <c r="K15" s="95" t="s">
+      <c r="I15" s="82"/>
+      <c r="J15" s="82" t="s">
+        <v>42</v>
+      </c>
+      <c r="K15" s="94"/>
+    </row>
+    <row r="16" spans="1:11" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="68">
+        <v>2</v>
+      </c>
+      <c r="B16" s="28" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="371.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="69">
-        <v>2</v>
-      </c>
-      <c r="B16" s="28" t="s">
+      <c r="C16" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="30" t="s">
+      <c r="F16" s="29" t="s">
         <v>40</v>
       </c>
       <c r="G16" s="27" t="s">
@@ -1664,50 +1926,52 @@
       <c r="J16" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="K16" s="29"/>
+      <c r="K16" s="94" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="17" spans="1:11" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="83">
+      <c r="A17" s="82">
         <v>3</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>45</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="83" t="s">
+      <c r="G17" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="H17" s="83" t="s">
+      <c r="H17" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="I17" s="83"/>
-      <c r="J17" s="83" t="s">
-        <v>50</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>53</v>
+      <c r="I17" s="82"/>
+      <c r="J17" s="82" t="s">
+        <v>42</v>
+      </c>
+      <c r="K17" s="94" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="89">
+      <c r="A18" s="88">
         <v>4</v>
       </c>
-      <c r="B18" s="89" t="s">
+      <c r="B18" s="88" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="80" t="s">
-        <v>69</v>
+      <c r="C18" s="79" t="s">
+        <v>66</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>47</v>
@@ -1716,85 +1980,83 @@
         <v>48</v>
       </c>
       <c r="F18" s="26"/>
-      <c r="G18" s="90" t="s">
+      <c r="G18" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="83"/>
-      <c r="I18" s="83"/>
-      <c r="J18" s="83"/>
+      <c r="H18" s="82"/>
+      <c r="I18" s="82"/>
+      <c r="J18" s="82"/>
       <c r="K18" s="14"/>
     </row>
-    <row r="19" spans="1:11" ht="352.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="89"/>
-      <c r="B19" s="89"/>
-      <c r="C19" s="81" t="s">
-        <v>70</v>
+    <row r="19" spans="1:11" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="88"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="80" t="s">
+        <v>67</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>49</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="92" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="89"/>
-      <c r="H19" s="83" t="s">
+      <c r="G19" s="88"/>
+      <c r="H19" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="I19" s="83"/>
-      <c r="J19" s="83" t="s">
-        <v>50</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>54</v>
+      <c r="I19" s="82"/>
+      <c r="J19" s="82" t="s">
+        <v>42</v>
+      </c>
+      <c r="K19" s="94" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="393.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="89"/>
-      <c r="B20" s="89"/>
-      <c r="C20" s="81" t="s">
+    <row r="20" spans="1:11" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="88"/>
+      <c r="B20" s="88"/>
+      <c r="C20" s="80" t="s">
         <v>52</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="93"/>
-      <c r="G20" s="89"/>
-      <c r="H20" s="83" t="s">
+      <c r="F20" s="92"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="I20" s="83"/>
-      <c r="J20" s="83" t="s">
-        <v>50</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>55</v>
-      </c>
+      <c r="I20" s="82"/>
+      <c r="J20" s="82" t="s">
+        <v>42</v>
+      </c>
+      <c r="K20" s="8"/>
     </row>
-    <row r="21" spans="1:11" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="89"/>
-      <c r="B21" s="89"/>
-      <c r="C21" s="82" t="s">
-        <v>71</v>
+    <row r="21" spans="1:11" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="88"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="81" t="s">
+        <v>68</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="93"/>
-      <c r="G21" s="89"/>
-      <c r="H21" s="83" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="92"/>
+      <c r="G21" s="88"/>
+      <c r="H21" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="I21" s="83"/>
-      <c r="J21" s="83" t="s">
+      <c r="I21" s="82"/>
+      <c r="J21" s="82" t="s">
         <v>42</v>
       </c>
       <c r="K21" s="14"/>
@@ -1823,5 +2085,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Approval of US20 Test Case
Reviewed and approved US20 Test Case system testing with signature
</commit_message>
<xml_diff>
--- a/SimpCity US20 Test Case.xlsx
+++ b/SimpCity US20 Test Case.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sem3.2-DevOps\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA04C30-378F-4569-9376-B7A7E6B13A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8004C81-91A6-497A-80D5-7E5FC31CE49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US20" sheetId="2" r:id="rId1"/>
@@ -938,36 +938,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1554,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22602A42-1986-4734-8038-194763616F21}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1589,24 +1589,24 @@
     </row>
     <row r="2" spans="1:11" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="47"/>
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="84"/>
+      <c r="C2" s="91"/>
       <c r="D2" s="16"/>
-      <c r="E2" s="86" t="s">
+      <c r="E2" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="84"/>
+      <c r="F2" s="91"/>
       <c r="G2" s="42"/>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="84"/>
-      <c r="J2" s="86" t="s">
+      <c r="I2" s="91"/>
+      <c r="J2" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="87"/>
+      <c r="K2" s="94"/>
     </row>
     <row r="3" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21"/>
@@ -1677,7 +1677,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="78" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G5" s="31"/>
       <c r="H5" s="34" t="s">
@@ -1722,27 +1722,27 @@
     </row>
     <row r="7" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21"/>
-      <c r="B7" s="85" t="s">
+      <c r="B7" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="85"/>
+      <c r="C7" s="92"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="85" t="s">
+      <c r="E7" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="85"/>
+      <c r="F7" s="92"/>
       <c r="G7" s="31"/>
-      <c r="H7" s="85" t="s">
+      <c r="H7" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="85"/>
+      <c r="I7" s="92"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="21"/>
       <c r="B8" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="93" t="s">
+      <c r="C8" s="84" t="s">
         <v>54</v>
       </c>
       <c r="D8" s="14"/>
@@ -1750,7 +1750,7 @@
         <v>27</v>
       </c>
       <c r="F8" s="72" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="G8" s="37"/>
       <c r="H8" s="73" t="s">
@@ -1771,7 +1771,7 @@
         <v>25</v>
       </c>
       <c r="F9" s="76" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="G9" s="31"/>
       <c r="H9" s="63" t="s">
@@ -1895,7 +1895,7 @@
       <c r="J15" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="K15" s="94"/>
+      <c r="K15" s="85"/>
     </row>
     <row r="16" spans="1:11" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="68">
@@ -1926,7 +1926,7 @@
       <c r="J16" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="K16" s="94" t="s">
+      <c r="K16" s="85" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1959,15 +1959,15 @@
       <c r="J17" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="K17" s="94" t="s">
+      <c r="K17" s="85" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="88">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="86">
         <v>4</v>
       </c>
-      <c r="B18" s="88" t="s">
+      <c r="B18" s="86" t="s">
         <v>46</v>
       </c>
       <c r="C18" s="79" t="s">
@@ -1980,7 +1980,7 @@
         <v>48</v>
       </c>
       <c r="F18" s="26"/>
-      <c r="G18" s="89" t="s">
+      <c r="G18" s="87" t="s">
         <v>41</v>
       </c>
       <c r="H18" s="82"/>
@@ -1989,8 +1989,8 @@
       <c r="K18" s="14"/>
     </row>
     <row r="19" spans="1:11" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="88"/>
-      <c r="B19" s="88"/>
+      <c r="A19" s="86"/>
+      <c r="B19" s="86"/>
       <c r="C19" s="80" t="s">
         <v>67</v>
       </c>
@@ -2000,10 +2000,10 @@
       <c r="E19" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F19" s="91" t="s">
+      <c r="F19" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="88"/>
+      <c r="G19" s="86"/>
       <c r="H19" s="82" t="s">
         <v>50</v>
       </c>
@@ -2011,13 +2011,13 @@
       <c r="J19" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="K19" s="94" t="s">
+      <c r="K19" s="85" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="88"/>
-      <c r="B20" s="88"/>
+      <c r="A20" s="86"/>
+      <c r="B20" s="86"/>
       <c r="C20" s="80" t="s">
         <v>52</v>
       </c>
@@ -2027,8 +2027,8 @@
       <c r="E20" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="92"/>
-      <c r="G20" s="88"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="86"/>
       <c r="H20" s="82" t="s">
         <v>42</v>
       </c>
@@ -2039,8 +2039,8 @@
       <c r="K20" s="8"/>
     </row>
     <row r="21" spans="1:11" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="88"/>
-      <c r="B21" s="88"/>
+      <c r="A21" s="86"/>
+      <c r="B21" s="86"/>
       <c r="C21" s="81" t="s">
         <v>68</v>
       </c>
@@ -2050,8 +2050,8 @@
       <c r="E21" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F21" s="92"/>
-      <c r="G21" s="88"/>
+      <c r="F21" s="89"/>
+      <c r="G21" s="86"/>
       <c r="H21" s="82" t="s">
         <v>42</v>
       </c>
@@ -2063,11 +2063,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="B1:C1"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="J2:K2"/>
@@ -2075,6 +2070,11 @@
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H15:J21" xr:uid="{4128DC36-7888-406E-9331-9EDDE928E7BC}">

</xml_diff>